<commit_message>
visor and children update based on delta
</commit_message>
<xml_diff>
--- a/core/assets/levels/tut9test.xlsx
+++ b/core/assets/levels/tut9test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\Git\MangoSnoopers\core\assets\levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762C5A1D-1A33-432D-846C-50D09F51008A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BFA94E-643B-42F8-87E9-6F9449503579}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="0" windowWidth="27855" windowHeight="12810" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2835" yWindow="0" windowWidth="27855" windowHeight="12810" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Region</t>
   </si>
@@ -293,6 +293,12 @@
   </si>
   <si>
     <t>Which blocks to use</t>
+  </si>
+  <si>
+    <t>Sun Start</t>
+  </si>
+  <si>
+    <t>rear enemy</t>
   </si>
 </sst>
 </file>
@@ -715,7 +721,7 @@
   <dimension ref="A1:AS1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1"/>
@@ -805,7 +811,9 @@
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
-      <c r="E3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="5"/>
       <c r="H3" s="3"/>
@@ -823,9 +831,7 @@
         <v>43</v>
       </c>
       <c r="D4" s="10"/>
-      <c r="E4" s="9" t="s">
-        <v>21</v>
-      </c>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:10" ht="16.5" customHeight="1">
       <c r="A5">
@@ -838,6 +844,9 @@
         <v>0</v>
       </c>
       <c r="D5" s="10"/>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" ht="16.5" customHeight="1">
@@ -845,6 +854,9 @@
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
+      <c r="E6" t="s">
+        <v>46</v>
+      </c>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" ht="16.5" customHeight="1">
@@ -970,7 +982,9 @@
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="F21" s="1"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>

</xml_diff>

<commit_message>
inArea fix, dvd drag to screen, radio mute fix
</commit_message>
<xml_diff>
--- a/core/assets/levels/tut9test.xlsx
+++ b/core/assets/levels/tut9test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\Git\MangoSnoopers\core\assets\levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5479168A-E24F-4B16-BE45-608A79466881}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44189411-2C9A-4AC0-8FFD-98CFFDA2E7F9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="0" windowWidth="27855" windowHeight="12810" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2835" yWindow="0" windowWidth="13365" windowHeight="12195" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
   <si>
     <t>Region</t>
   </si>
@@ -299,6 +299,21 @@
   </si>
   <si>
     <t>gnome</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>rustling_leaves.mp3</t>
+  </si>
+  <si>
+    <t>Jazz</t>
+  </si>
+  <si>
+    <t>bensound-thejazzpiano.mp3</t>
   </si>
 </sst>
 </file>
@@ -721,7 +736,7 @@
   <dimension ref="A1:AS1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1"/>
@@ -883,6 +898,12 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" ht="16.5" customHeight="1">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="H9" t="s">
@@ -891,6 +912,12 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" ht="16.5" customHeight="1">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="J10" s="2"/>
@@ -1017,7 +1044,9 @@
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
-      <c r="E22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="F22" s="2"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>

</xml_diff>